<commit_message>
added audio and video to example
</commit_message>
<xml_diff>
--- a/slideshows.xlsx
+++ b/slideshows.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicco Garofalo\Documents\Husky Undergrad\Research\dwelltime-outline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD3DF46-32AD-4550-9F9D-4A1A20D4F93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52505FCD-475B-414F-943B-9BB08D59050B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FE25C0E6-6A6C-46DE-953E-EB5C7B6ADE79}"/>
+    <workbookView xWindow="6570" yWindow="2580" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{FE25C0E6-6A6C-46DE-953E-EB5C7B6ADE79}"/>
   </bookViews>
   <sheets>
     <sheet name="card-trick" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="279">
   <si>
     <t>fileName</t>
   </si>
@@ -861,6 +861,18 @@
   </si>
   <si>
     <t>options</t>
+  </si>
+  <si>
+    <t>jump-07-0.mp4</t>
+  </si>
+  <si>
+    <t>ding.mp3</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>{"trial_ends_after_audio":true}</t>
   </si>
 </sst>
 </file>
@@ -2575,10 +2587,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA469DC-D02F-41BC-916D-C4872F0B783D}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2596,59 +2608,75 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>260</v>
+        <v>276</v>
+      </c>
+      <c r="C2" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>272</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>269</v>
       </c>
     </row>

</xml_diff>

<commit_message>
don't parse null values
</commit_message>
<xml_diff>
--- a/slideshows.xlsx
+++ b/slideshows.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicco Garofalo\Documents\Husky Undergrad\Research\dwelltime-outline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52505FCD-475B-414F-943B-9BB08D59050B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14A76A-D620-4863-8C09-018F56A1F9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6570" yWindow="2580" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{FE25C0E6-6A6C-46DE-953E-EB5C7B6ADE79}"/>
   </bookViews>
@@ -2590,7 +2590,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
tried to get methods to trigger
</commit_message>
<xml_diff>
--- a/slideshows.xlsx
+++ b/slideshows.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicco Garofalo\Documents\Husky Undergrad\Research\dwelltime-outline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14A76A-D620-4863-8C09-018F56A1F9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19218807-90BA-4A02-886D-4BB478DCB511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6570" yWindow="2580" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{FE25C0E6-6A6C-46DE-953E-EB5C7B6ADE79}"/>
   </bookViews>
@@ -872,7 +872,7 @@
     <t>image</t>
   </si>
   <si>
-    <t>{"trial_ends_after_audio":true}</t>
+    <t>{"trial_ends_after_audio":true,"prompt":"Audio is playing right now, wait a moment."}</t>
   </si>
 </sst>
 </file>
@@ -2590,7 +2590,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A2:A4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "tried to get methods to trigger"
This reverts commit db0eebbb658b1de4a3adb338d0a4c227403f799e
</commit_message>
<xml_diff>
--- a/slideshows.xlsx
+++ b/slideshows.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicco Garofalo\Documents\Husky Undergrad\Research\dwelltime-outline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19218807-90BA-4A02-886D-4BB478DCB511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14A76A-D620-4863-8C09-018F56A1F9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6570" yWindow="2580" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{FE25C0E6-6A6C-46DE-953E-EB5C7B6ADE79}"/>
   </bookViews>
@@ -872,7 +872,7 @@
     <t>image</t>
   </si>
   <si>
-    <t>{"trial_ends_after_audio":true,"prompt":"Audio is playing right now, wait a moment."}</t>
+    <t>{"trial_ends_after_audio":true}</t>
   </si>
 </sst>
 </file>
@@ -2590,7 +2590,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A4" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>